<commit_message>
Add RecordID field to source files.
</commit_message>
<xml_diff>
--- a/migrate_upload/examples/TW_2013_GOEA_Owyhee--with_Notes.xlsx
+++ b/migrate_upload/examples/TW_2013_GOEA_Owyhee--with_Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="2475" windowWidth="24285" windowHeight="8085"/>
+    <workbookView xWindow="1050" yWindow="2535" windowWidth="24240" windowHeight="8025" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DataEntry" sheetId="2" r:id="rId1"/>
@@ -60,8 +60,52 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>nwade</author>
+  </authors>
+  <commentList>
+    <comment ref="AQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>nwade:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Enter an identifying ID number of your photo.  Submit digital copies of photos, titled with your given ID. </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Leave this field null if no photos were taken.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="216">
   <si>
     <t>Territory</t>
   </si>
@@ -850,6 +894,9 @@
   </si>
   <si>
     <t>first.last@idfg.idaho.gov</t>
+  </si>
+  <si>
+    <t>RecordID</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1595,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1696,6 +1743,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="16" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2053,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="AM12" workbookViewId="0">
+      <selection activeCell="AR38" sqref="A14:AR38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2627,17 +2677,17 @@
       <c r="Q13" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="89" t="s">
+      <c r="R13" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="S13" s="89"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="90"/>
-      <c r="X13" s="90"/>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="90"/>
+      <c r="S13" s="90"/>
+      <c r="T13" s="91"/>
+      <c r="U13" s="91"/>
+      <c r="V13" s="91"/>
+      <c r="W13" s="91"/>
+      <c r="X13" s="91"/>
+      <c r="Y13" s="91"/>
+      <c r="Z13" s="91"/>
       <c r="AA13" s="67" t="s">
         <v>25</v>
       </c>
@@ -4702,8 +4752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5026,7 +5076,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5268,1791 +5318,2424 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:45" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="68" t="s">
         <v>135</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="68" t="s">
         <v>136</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="68" t="s">
         <v>137</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="68" t="s">
         <v>142</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="60" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="AS1" s="89" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="L2">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="35">
         <v>41445</v>
       </c>
-      <c r="O2" t="s">
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="36">
         <v>43.382463000000001</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="36">
         <v>-116.870228</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="AS2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L3">
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="35">
         <v>41398</v>
       </c>
-      <c r="O3" t="s">
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="76">
         <v>42.812181000000002</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="76">
         <v>-116.450751</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="31"/>
+      <c r="AL3" s="31"/>
+      <c r="AM3" s="31"/>
+      <c r="AN3" s="31"/>
+      <c r="AO3" s="31"/>
+      <c r="AP3" s="31"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="AS3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L4">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="35">
         <v>41404</v>
       </c>
-      <c r="O4" t="s">
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="71"/>
+      <c r="W4" s="71"/>
+      <c r="X4" s="71"/>
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="76">
         <v>42.7866</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="76">
         <v>-116.49314200000001</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AD4" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AE4" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AI4" s="31"/>
+      <c r="AJ4" s="31"/>
+      <c r="AK4" s="31"/>
+      <c r="AL4" s="31"/>
+      <c r="AM4" s="31"/>
+      <c r="AN4" s="31"/>
+      <c r="AO4" s="31"/>
+      <c r="AP4" s="31"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="AS4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L5">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="35">
         <v>41415</v>
       </c>
-      <c r="O5" t="s">
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
+      <c r="Y5" s="71"/>
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="76">
         <v>42.795667000000002</v>
       </c>
-      <c r="AC5">
+      <c r="AC5" s="76">
         <v>-116.501904</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AD5" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AE5" s="74" t="s">
         <v>155</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AI5" s="31"/>
+      <c r="AJ5" s="31"/>
+      <c r="AK5" s="31"/>
+      <c r="AL5" s="31"/>
+      <c r="AM5" s="31"/>
+      <c r="AN5" s="31"/>
+      <c r="AO5" s="31"/>
+      <c r="AP5" s="31"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="AS5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L6">
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="35">
         <v>41419</v>
       </c>
-      <c r="O6" t="s">
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71"/>
+      <c r="X6" s="71"/>
+      <c r="Y6" s="71"/>
+      <c r="Z6" s="71"/>
+      <c r="AA6" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="76">
         <v>42.814708000000003</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="76">
         <v>-116.55018800000001</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AE6" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AI6" s="31"/>
+      <c r="AJ6" s="31"/>
+      <c r="AK6" s="31"/>
+      <c r="AL6" s="31"/>
+      <c r="AM6" s="31"/>
+      <c r="AN6" s="31"/>
+      <c r="AO6" s="31"/>
+      <c r="AP6" s="31"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="AS6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L7">
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="35">
         <v>41362</v>
       </c>
-      <c r="O7" t="s">
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB7">
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="71"/>
+      <c r="X7" s="71"/>
+      <c r="Y7" s="71"/>
+      <c r="Z7" s="71"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="73">
         <v>42.9352852731</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" s="73">
         <v>-116.384567434</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AD7" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AE7" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AI7" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ7">
+      <c r="AJ7" s="72">
         <v>60</v>
       </c>
-      <c r="AK7">
+      <c r="AK7" s="31">
         <v>150</v>
       </c>
-      <c r="AL7">
+      <c r="AL7" s="31">
         <v>150</v>
       </c>
-      <c r="AM7">
+      <c r="AM7" s="31">
         <v>1</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AN7" s="31" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="AO7" s="31"/>
+      <c r="AP7" s="31"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L8">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="35">
         <v>41362</v>
       </c>
-      <c r="O8" t="s">
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB8">
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="71"/>
+      <c r="Z8" s="71"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="73">
         <v>42.9352852731</v>
       </c>
-      <c r="AC8">
+      <c r="AC8" s="73">
         <v>-116.384567434</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AD8" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AE8" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AI8" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ8">
+      <c r="AJ8" s="72">
         <v>60</v>
       </c>
-      <c r="AK8">
+      <c r="AK8" s="31">
         <v>150</v>
       </c>
-      <c r="AL8">
+      <c r="AL8" s="31">
         <v>150</v>
       </c>
-      <c r="AM8">
+      <c r="AM8" s="31">
         <v>1</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AN8" s="31" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="AO8" s="31"/>
+      <c r="AP8" s="31"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L9">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="35">
         <v>41367</v>
       </c>
-      <c r="O9" t="s">
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB9">
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+      <c r="U9" s="71"/>
+      <c r="V9" s="71"/>
+      <c r="W9" s="71"/>
+      <c r="X9" s="71"/>
+      <c r="Y9" s="71"/>
+      <c r="Z9" s="71"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="73">
         <v>42.938184415199999</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" s="73">
         <v>-116.38055538499999</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AD9" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AE9" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AI9" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="31">
         <v>45</v>
       </c>
-      <c r="AK9">
+      <c r="AK9" s="31">
         <v>150</v>
       </c>
-      <c r="AL9">
+      <c r="AL9" s="31">
         <v>150</v>
       </c>
-      <c r="AM9">
+      <c r="AM9" s="31">
         <v>1</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AN9" s="31" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="AO9" s="31"/>
+      <c r="AP9" s="31"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L10">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="35">
         <v>41367</v>
       </c>
-      <c r="O10" t="s">
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB10">
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="71"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="71"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="71"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="73">
         <v>42.938184415199999</v>
       </c>
-      <c r="AC10">
+      <c r="AC10" s="73">
         <v>-116.38055538499999</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AD10" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AE10" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AI10" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ10">
+      <c r="AJ10" s="31">
         <v>45</v>
       </c>
-      <c r="AK10">
+      <c r="AK10" s="31">
         <v>150</v>
       </c>
-      <c r="AL10">
+      <c r="AL10" s="31">
         <v>150</v>
       </c>
-      <c r="AM10">
+      <c r="AM10" s="31">
         <v>1</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AN10" s="31" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="AO10" s="31"/>
+      <c r="AP10" s="31"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L11">
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="35">
         <v>41368</v>
       </c>
-      <c r="O11" t="s">
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB11">
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="71"/>
+      <c r="Y11" s="71"/>
+      <c r="Z11" s="71"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="73">
         <v>42.926680380299999</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="73">
         <v>-116.391331874</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AD11" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AE11" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AI11" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ11">
+      <c r="AJ11" s="31">
         <v>50</v>
       </c>
-      <c r="AK11">
+      <c r="AK11" s="31">
         <v>0</v>
       </c>
-      <c r="AL11">
+      <c r="AL11" s="31">
         <v>0</v>
       </c>
-      <c r="AM11">
+      <c r="AM11" s="31">
         <v>1.5</v>
       </c>
-      <c r="AN11" t="s">
+      <c r="AN11" s="31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="AO11" s="31"/>
+      <c r="AP11" s="31"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L12">
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="35">
         <v>41368</v>
       </c>
-      <c r="O12" t="s">
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB12">
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="71"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="71"/>
+      <c r="Y12" s="71"/>
+      <c r="Z12" s="71"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="73">
         <v>42.926680380299999</v>
       </c>
-      <c r="AC12">
+      <c r="AC12" s="73">
         <v>-116.391331874</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AD12" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AE12" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AI12" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ12">
+      <c r="AJ12" s="31">
         <v>50</v>
       </c>
-      <c r="AK12">
+      <c r="AK12" s="31">
         <v>45</v>
       </c>
-      <c r="AL12">
+      <c r="AL12" s="31">
         <v>45</v>
       </c>
-      <c r="AM12">
+      <c r="AM12" s="31">
         <v>1</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AN12" s="31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="AO12" s="31"/>
+      <c r="AP12" s="31"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L13">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="35">
         <v>41368</v>
       </c>
-      <c r="O13" t="s">
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB13">
+      <c r="S13" s="71"/>
+      <c r="T13" s="71"/>
+      <c r="U13" s="71"/>
+      <c r="V13" s="71"/>
+      <c r="W13" s="71"/>
+      <c r="X13" s="71"/>
+      <c r="Y13" s="71"/>
+      <c r="Z13" s="71"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="76">
         <v>42.927233999999999</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" s="76">
         <v>-116.391098</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AD13" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AE13" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AI13" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="31">
         <v>50</v>
       </c>
-      <c r="AK13">
+      <c r="AK13" s="31">
         <v>200</v>
       </c>
-      <c r="AL13">
+      <c r="AL13" s="31">
         <v>200</v>
       </c>
-      <c r="AM13">
+      <c r="AM13" s="31">
         <v>0.5</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AN13" s="31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="AO13" s="31"/>
+      <c r="AP13" s="31"/>
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="9"/>
+      <c r="AS13" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14" s="9"/>
+      <c r="I14" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L14">
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="35">
         <v>41414</v>
       </c>
-      <c r="O14" t="s">
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB14">
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="71"/>
+      <c r="V14" s="71"/>
+      <c r="W14" s="71"/>
+      <c r="X14" s="71"/>
+      <c r="Y14" s="71"/>
+      <c r="Z14" s="71"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="73">
         <v>42.800057023599997</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" s="73">
         <v>-116.471774783</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AD14" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AE14" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AF14" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AI14" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" s="31">
         <v>20</v>
       </c>
-      <c r="AK14">
+      <c r="AK14" s="31">
         <v>280</v>
       </c>
-      <c r="AL14">
+      <c r="AL14" s="31">
         <v>280</v>
       </c>
-      <c r="AM14">
+      <c r="AM14" s="31">
         <v>1</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AN14" s="31" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="AO14" s="31"/>
+      <c r="AP14" s="31"/>
+      <c r="AQ14" s="9"/>
+      <c r="AR14" s="9"/>
+      <c r="AS14" s="31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L15">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="35">
         <v>41415</v>
       </c>
-      <c r="O15" t="s">
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="AB15">
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="71"/>
+      <c r="V15" s="71"/>
+      <c r="W15" s="71"/>
+      <c r="X15" s="71"/>
+      <c r="Y15" s="71"/>
+      <c r="Z15" s="71"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="73">
         <v>42.795199424400003</v>
       </c>
-      <c r="AC15">
+      <c r="AC15" s="73">
         <v>-116.504983182</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AD15" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AE15" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH15" t="s">
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AI15" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ15">
+      <c r="AJ15" s="31">
         <v>14</v>
       </c>
-      <c r="AK15">
+      <c r="AK15" s="31">
         <v>160</v>
       </c>
-      <c r="AL15">
+      <c r="AL15" s="31">
         <v>160</v>
       </c>
-      <c r="AM15">
+      <c r="AM15" s="31">
         <v>0.5</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AN15" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="AR15" t="s">
+      <c r="AO15" s="31"/>
+      <c r="AP15" s="31"/>
+      <c r="AQ15" s="9"/>
+      <c r="AR15" s="9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="AS15" s="31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L16">
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="35">
         <v>41415</v>
       </c>
-      <c r="O16" t="s">
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="AB16">
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="71"/>
+      <c r="V16" s="71"/>
+      <c r="W16" s="71"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="73">
         <v>42.795222138600003</v>
       </c>
-      <c r="AC16">
+      <c r="AC16" s="73">
         <v>-116.50400160300001</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AD16" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AE16" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI16" t="s">
+      <c r="AI16" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ16">
+      <c r="AJ16" s="31">
         <v>14</v>
       </c>
-      <c r="AK16">
+      <c r="AK16" s="31">
         <v>160</v>
       </c>
-      <c r="AL16">
+      <c r="AL16" s="31">
         <v>160</v>
       </c>
-      <c r="AM16">
+      <c r="AM16" s="31">
         <v>0.5</v>
       </c>
-      <c r="AN16" t="s">
+      <c r="AN16" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="AR16" t="s">
+      <c r="AO16" s="31"/>
+      <c r="AP16" s="31"/>
+      <c r="AQ16" s="9"/>
+      <c r="AR16" s="9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="AS16" s="31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="L17">
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="35">
         <v>41428</v>
       </c>
-      <c r="O17" t="s">
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB17">
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="71"/>
+      <c r="W17" s="71"/>
+      <c r="X17" s="71"/>
+      <c r="Y17" s="71"/>
+      <c r="Z17" s="71"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="73">
         <v>43.312926569200002</v>
       </c>
-      <c r="AC17">
+      <c r="AC17" s="73">
         <v>-116.695286356</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AD17" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AE17" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH17" t="s">
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI17" t="s">
+      <c r="AI17" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AN17" t="s">
+      <c r="AJ17" s="31"/>
+      <c r="AK17" s="31"/>
+      <c r="AL17" s="31"/>
+      <c r="AM17" s="31"/>
+      <c r="AN17" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="AR17" t="s">
+      <c r="AO17" s="31"/>
+      <c r="AP17" s="31"/>
+      <c r="AQ17" s="9"/>
+      <c r="AR17" s="9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="AS17" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="L18">
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="35">
         <v>41428</v>
       </c>
-      <c r="O18" t="s">
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q18" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB18">
+      <c r="S18" s="71"/>
+      <c r="T18" s="71"/>
+      <c r="U18" s="71"/>
+      <c r="V18" s="71"/>
+      <c r="W18" s="71"/>
+      <c r="X18" s="71"/>
+      <c r="Y18" s="71"/>
+      <c r="Z18" s="71"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="73">
         <v>43.313096795299998</v>
       </c>
-      <c r="AC18">
+      <c r="AC18" s="73">
         <v>-116.69558038300001</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AD18" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AE18" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AI18" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AJ18" s="31"/>
+      <c r="AK18" s="31"/>
+      <c r="AL18" s="31"/>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="AR18" t="s">
+      <c r="AO18" s="31"/>
+      <c r="AP18" s="31"/>
+      <c r="AQ18" s="9"/>
+      <c r="AR18" s="9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="AS18" s="31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="L19">
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="35">
         <v>41428</v>
       </c>
-      <c r="O19" t="s">
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q19" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB19">
+      <c r="S19" s="71"/>
+      <c r="T19" s="71"/>
+      <c r="U19" s="71"/>
+      <c r="V19" s="71"/>
+      <c r="W19" s="71"/>
+      <c r="X19" s="71"/>
+      <c r="Y19" s="71"/>
+      <c r="Z19" s="71"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="73">
         <v>43.313700324300001</v>
       </c>
-      <c r="AC19">
+      <c r="AC19" s="73">
         <v>-116.69558038300001</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AD19" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AE19" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AI19" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="AJ19" s="31"/>
+      <c r="AK19" s="31"/>
+      <c r="AL19" s="31"/>
+      <c r="AM19" s="31"/>
+      <c r="AN19" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="AR19" t="s">
+      <c r="AO19" s="31"/>
+      <c r="AP19" s="31"/>
+      <c r="AQ19" s="9"/>
+      <c r="AR19" s="9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="AS19" s="31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="L20">
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="35">
         <v>41428</v>
       </c>
-      <c r="O20" t="s">
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q20" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB20">
+      <c r="S20" s="71"/>
+      <c r="T20" s="71"/>
+      <c r="U20" s="71"/>
+      <c r="V20" s="71"/>
+      <c r="W20" s="71"/>
+      <c r="X20" s="71"/>
+      <c r="Y20" s="71"/>
+      <c r="Z20" s="71"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="73">
         <v>43.314017563900002</v>
       </c>
-      <c r="AC20">
+      <c r="AC20" s="73">
         <v>-116.695472057</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AD20" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AE20" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI20" t="s">
+      <c r="AI20" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AN20" t="s">
+      <c r="AJ20" s="31"/>
+      <c r="AK20" s="31"/>
+      <c r="AL20" s="31"/>
+      <c r="AM20" s="31"/>
+      <c r="AN20" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="AR20" t="s">
+      <c r="AO20" s="31"/>
+      <c r="AP20" s="31"/>
+      <c r="AQ20" s="9"/>
+      <c r="AR20" s="9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="AS20" s="31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H21" s="9"/>
+      <c r="I21" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L21">
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="35">
         <v>41431</v>
       </c>
-      <c r="O21" t="s">
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB21">
+      <c r="S21" s="71"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="71"/>
+      <c r="V21" s="71"/>
+      <c r="W21" s="71"/>
+      <c r="X21" s="71"/>
+      <c r="Y21" s="71"/>
+      <c r="Z21" s="71"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="73">
         <v>42.935566745999999</v>
       </c>
-      <c r="AC21">
+      <c r="AC21" s="73">
         <v>-116.382071346</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AD21" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE21" t="s">
+      <c r="AE21" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH21" t="s">
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI21" t="s">
+      <c r="AI21" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ21">
+      <c r="AJ21" s="31">
         <v>50</v>
       </c>
-      <c r="AN21" t="s">
+      <c r="AK21" s="31"/>
+      <c r="AL21" s="31"/>
+      <c r="AM21" s="31"/>
+      <c r="AN21" s="31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="AO21" s="31"/>
+      <c r="AP21" s="31"/>
+      <c r="AQ21" s="9"/>
+      <c r="AR21" s="9"/>
+      <c r="AS21" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L22">
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="35">
         <v>41431</v>
       </c>
-      <c r="O22" t="s">
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB22">
+      <c r="S22" s="71"/>
+      <c r="T22" s="71"/>
+      <c r="U22" s="71"/>
+      <c r="V22" s="71"/>
+      <c r="W22" s="71"/>
+      <c r="X22" s="71"/>
+      <c r="Y22" s="71"/>
+      <c r="Z22" s="71"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="73">
         <v>42.935654751599998</v>
       </c>
-      <c r="AC22">
+      <c r="AC22" s="73">
         <v>-116.38195350300001</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AD22" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AE22" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AI22" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ22">
+      <c r="AJ22" s="31">
         <v>50</v>
       </c>
-      <c r="AN22" t="s">
+      <c r="AK22" s="31"/>
+      <c r="AL22" s="31"/>
+      <c r="AM22" s="31"/>
+      <c r="AN22" s="31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="AO22" s="31"/>
+      <c r="AP22" s="31"/>
+      <c r="AQ22" s="9"/>
+      <c r="AR22" s="9"/>
+      <c r="AS22" s="31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I23" t="s">
+      <c r="H23" s="9"/>
+      <c r="I23" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L23">
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="35">
         <v>41431</v>
       </c>
-      <c r="O23" t="s">
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB23">
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
+      <c r="U23" s="71"/>
+      <c r="V23" s="71"/>
+      <c r="W23" s="71"/>
+      <c r="X23" s="71"/>
+      <c r="Y23" s="71"/>
+      <c r="Z23" s="71"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="73">
         <v>42.936095658699998</v>
       </c>
-      <c r="AC23">
+      <c r="AC23" s="73">
         <v>-116.381118407</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AD23" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE23" t="s">
+      <c r="AE23" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH23" t="s">
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI23" t="s">
+      <c r="AI23" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ23">
+      <c r="AJ23" s="31">
         <v>50</v>
       </c>
-      <c r="AN23" t="s">
+      <c r="AK23" s="31"/>
+      <c r="AL23" s="31"/>
+      <c r="AM23" s="31"/>
+      <c r="AN23" s="31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="AO23" s="31"/>
+      <c r="AP23" s="31"/>
+      <c r="AQ23" s="9"/>
+      <c r="AR23" s="9"/>
+      <c r="AS23" s="31">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I24" t="s">
+      <c r="H24" s="9"/>
+      <c r="I24" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="L24">
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="35">
         <v>41431</v>
       </c>
-      <c r="O24" t="s">
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB24">
+      <c r="S24" s="71"/>
+      <c r="T24" s="71"/>
+      <c r="U24" s="71"/>
+      <c r="V24" s="71"/>
+      <c r="W24" s="71"/>
+      <c r="X24" s="71"/>
+      <c r="Y24" s="71"/>
+      <c r="Z24" s="71"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="73">
         <v>42.937620313899998</v>
       </c>
-      <c r="AC24">
+      <c r="AC24" s="73">
         <v>-116.380049063</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AD24" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AE24" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="AH24" t="s">
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI24" t="s">
+      <c r="AI24" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ24">
+      <c r="AJ24" s="31">
         <v>50</v>
       </c>
-      <c r="AN24" t="s">
+      <c r="AK24" s="31"/>
+      <c r="AL24" s="31"/>
+      <c r="AM24" s="31"/>
+      <c r="AN24" s="31" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="AO24" s="31"/>
+      <c r="AP24" s="31"/>
+      <c r="AQ24" s="9"/>
+      <c r="AR24" s="9"/>
+      <c r="AS24" s="31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I25" t="s">
+      <c r="H25" s="9"/>
+      <c r="I25" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="L25">
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="35">
         <v>41445</v>
       </c>
-      <c r="O25" t="s">
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="AB25">
+      <c r="S25" s="71"/>
+      <c r="T25" s="71"/>
+      <c r="U25" s="71"/>
+      <c r="V25" s="71"/>
+      <c r="W25" s="71"/>
+      <c r="X25" s="71"/>
+      <c r="Y25" s="71"/>
+      <c r="Z25" s="71"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="36">
         <v>43.40175</v>
       </c>
-      <c r="AC25">
+      <c r="AC25" s="76">
         <v>-116.851462</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AD25" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="AE25" t="s">
+      <c r="AE25" s="74" t="s">
         <v>155</v>
       </c>
-      <c r="AH25" t="s">
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="AI25" t="s">
+      <c r="AI25" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AJ25">
+      <c r="AJ25" s="31">
         <v>25</v>
       </c>
-      <c r="AN25" t="s">
+      <c r="AK25" s="31"/>
+      <c r="AL25" s="31"/>
+      <c r="AM25" s="31"/>
+      <c r="AN25" s="31" t="s">
         <v>165</v>
       </c>
+      <c r="AO25" s="31"/>
+      <c r="AP25" s="31"/>
+      <c r="AQ25" s="9"/>
+      <c r="AR25" s="9"/>
+      <c r="AS25" s="31">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
+    <hyperlink ref="E16" r:id="rId15"/>
+    <hyperlink ref="E17" r:id="rId16"/>
+    <hyperlink ref="E18" r:id="rId17"/>
+    <hyperlink ref="E19" r:id="rId18"/>
+    <hyperlink ref="E20" r:id="rId19"/>
+    <hyperlink ref="E21" r:id="rId20"/>
+    <hyperlink ref="E22" r:id="rId21"/>
+    <hyperlink ref="E23" r:id="rId22"/>
+    <hyperlink ref="E24" r:id="rId23"/>
+    <hyperlink ref="E25" r:id="rId24"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>